<commit_message>
Functionality for finding the number of afferent and efferent couplings has been implemented
</commit_message>
<xml_diff>
--- a/sheets/xlsxFiles.xlsx
+++ b/sheets/xlsxFiles.xlsx
@@ -421,7 +421,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\EntryPositionsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/EntryPositionsManager.sol</v>
       </c>
       <c r="B2">
         <v>296</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\ExitPositionsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/ExitPositionsManager.sol</v>
       </c>
       <c r="B3">
         <v>715</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\IncentivesVault.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/IncentivesVault.sol</v>
       </c>
       <c r="B4">
         <v>151</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\InterestRatesManager.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/InterestRatesManager.sol</v>
       </c>
       <c r="B5">
         <v>189</v>
@@ -489,16 +489,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IAaveIncentivesController.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/MatchingEngine.sol</v>
       </c>
       <c r="B6">
-        <v>154</v>
+        <v>354</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -506,16 +506,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IAToken.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/Morpho.sol</v>
       </c>
       <c r="B7">
-        <v>91</v>
+        <v>245</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -523,78 +523,78 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IERC20.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/MorphoGovernance.sol</v>
       </c>
       <c r="B8">
-        <v>81</v>
+        <v>531</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\ILendingPool.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/MorphoStorage.sol</v>
       </c>
       <c r="B9">
-        <v>418</v>
+        <v>87</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\ILendingPoolAddressesProvider.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/MorphoUtils.sol</v>
       </c>
       <c r="B10">
-        <v>61</v>
+        <v>338</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IPriceOracleGetter.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/PositionsManagerUtils.sol</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IScaledBalanceToken.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IEntryPositionsManager.sol</v>
       </c>
       <c r="B12">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -608,16 +608,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\aave\IVariableDebtToken.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IExitPositionsManager.sol</v>
       </c>
       <c r="B13">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -625,10 +625,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IEntryPositionsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IGetterUnderlyingAsset.sol</v>
       </c>
       <c r="B14">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -642,16 +642,16 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IExitPositionsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IIncentivesVault.sol</v>
       </c>
       <c r="B15">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IGetterUnderlyingAsset.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IInterestRatesManager.sol</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -676,16 +676,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IIncentivesVault.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IMorpho.sol</v>
       </c>
       <c r="B17">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IInterestRatesManager.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IOracle.sol</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -710,16 +710,16 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IMorpho.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/IRewardsManager.sol</v>
       </c>
       <c r="B19">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -727,16 +727,16 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IOracle.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/IAToken.sol</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -744,16 +744,16 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\IRewardsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/IAaveIncentivesController.sol</v>
       </c>
       <c r="B21">
-        <v>27</v>
+        <v>154</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -761,10 +761,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\interfaces\lido\ILido.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/IERC20.sol</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -778,16 +778,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\IndexesLens.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/ILendingPool.sol</v>
       </c>
       <c r="B23">
-        <v>126</v>
+        <v>418</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -795,16 +795,16 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\interfaces\ILens.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/ILendingPoolAddressesProvider.sol</v>
       </c>
       <c r="B24">
-        <v>257</v>
+        <v>61</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -812,16 +812,16 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\Lens.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/IPriceOracleGetter.sol</v>
       </c>
       <c r="B25">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -829,27 +829,27 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\LensStorage.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/IScaledBalanceToken.sol</v>
       </c>
       <c r="B26">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\MarketsLens.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/aave/IVariableDebtToken.sol</v>
       </c>
       <c r="B27">
-        <v>235</v>
+        <v>79</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -863,16 +863,16 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\RatesLens.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/interfaces/lido/ILido.sol</v>
       </c>
       <c r="B28">
-        <v>469</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -880,33 +880,33 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\lens\UsersLens.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/lens/IndexesLens.sol</v>
       </c>
       <c r="B29">
-        <v>483</v>
+        <v>126</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\DataTypes.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/lens/Lens.sol</v>
       </c>
       <c r="B30">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -914,33 +914,33 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\Errors.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/lens/LensStorage.sol</v>
       </c>
       <c r="B31">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\ReserveConfiguration.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/lens/MarketsLens.sol</v>
       </c>
       <c r="B32">
-        <v>376</v>
+        <v>235</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -948,16 +948,16 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\aave\UserConfiguration.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/lens/RatesLens.sol</v>
       </c>
       <c r="B33">
-        <v>17</v>
+        <v>469</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -965,10 +965,10 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\InterestRatesModel.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/lens/UsersLens.sol</v>
       </c>
       <c r="B34">
-        <v>207</v>
+        <v>483</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -977,21 +977,21 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\libraries\Types.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/lens/interfaces/ILens.sol</v>
       </c>
       <c r="B35">
-        <v>105</v>
+        <v>257</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -999,10 +999,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MatchingEngine.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/libraries/InterestRatesModel.sol</v>
       </c>
       <c r="B36">
-        <v>354</v>
+        <v>207</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1011,21 +1011,21 @@
         <v>1</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\Morpho.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/libraries/Types.sol</v>
       </c>
       <c r="B37">
-        <v>245</v>
+        <v>105</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1033,75 +1033,75 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MorphoGovernance.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/libraries/aave/DataTypes.sol</v>
       </c>
       <c r="B38">
-        <v>531</v>
+        <v>54</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MorphoStorage.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/libraries/aave/Errors.sol</v>
       </c>
       <c r="B39">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\MorphoUtils.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/libraries/aave/ReserveConfiguration.sol</v>
       </c>
       <c r="B40">
-        <v>338</v>
+        <v>376</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>morpho\morpho-v1-main\src\aave-v2\PositionsManagerUtils.sol</v>
+        <v>morpho/morpho-v1-main/src/aave-v2/libraries/aave/UserConfiguration.sol</v>
       </c>
       <c r="B41">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>morpho\morpho-v1-main\src\common\rewards-distribution\RewardsDistributor.sol</v>
+        <v>morpho/morpho-v1-main/src/common/rewards-distribution/RewardsDistributor.sol</v>
       </c>
       <c r="B42">
         <v>104</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>morpho\morpho-v1-main\src\common\test\FakeToken.sol</v>
+        <v>morpho/morpho-v1-main/src/common/test/FakeToken.sol</v>
       </c>
       <c r="B43">
         <v>13</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>morpho\morpho-v1-main\src\compound\IncentivesVault.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/IncentivesVault.sol</v>
       </c>
       <c r="B44">
         <v>156</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>morpho\morpho-v1-main\src\compound\InterestRatesManager.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/InterestRatesManager.sol</v>
       </c>
       <c r="B45">
         <v>171</v>
@@ -1169,16 +1169,16 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\compound\ICompound.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/MatchingEngine.sol</v>
       </c>
       <c r="B46">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1186,10 +1186,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IIncentivesVault.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/Morpho.sol</v>
       </c>
       <c r="B47">
-        <v>29</v>
+        <v>247</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IInterestRatesManager.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/MorphoGovernance.sol</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>487</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -1220,50 +1220,50 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IMorpho.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/MorphoStorage.sol</v>
       </c>
       <c r="B49">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IOracle.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/MorphoUtils.sol</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>227</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IPositionsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/PositionsManager.sol</v>
       </c>
       <c r="B51">
-        <v>44</v>
+        <v>1032</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1271,33 +1271,33 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IRewardsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/RewardsManager.sol</v>
       </c>
       <c r="B52">
-        <v>39</v>
+        <v>262</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>morpho\morpho-v1-main\src\compound\interfaces\IWETH.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/IIncentivesVault.sol</v>
       </c>
       <c r="B53">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1305,16 +1305,16 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\IndexesLens.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/IInterestRatesManager.sol</v>
       </c>
       <c r="B54">
-        <v>159</v>
+        <v>7</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1322,16 +1322,16 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\interfaces\ILens.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/IMorpho.sol</v>
       </c>
       <c r="B55">
-        <v>291</v>
+        <v>88</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1339,16 +1339,16 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\Lens.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/IOracle.sol</v>
       </c>
       <c r="B56">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1356,27 +1356,27 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\LensStorage.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/IPositionsManager.sol</v>
       </c>
       <c r="B57">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\MarketsLens.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/IRewardsManager.sol</v>
       </c>
       <c r="B58">
-        <v>180</v>
+        <v>39</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1390,16 +1390,16 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\RatesLens.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/IWETH.sol</v>
       </c>
       <c r="B59">
-        <v>453</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -1407,16 +1407,16 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\RewardsLens.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/interfaces/compound/ICompound.sol</v>
       </c>
       <c r="B60">
-        <v>181</v>
+        <v>380</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -1424,16 +1424,16 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>morpho\morpho-v1-main\src\compound\lens\UsersLens.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/IndexesLens.sol</v>
       </c>
       <c r="B61">
-        <v>471</v>
+        <v>159</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -1441,16 +1441,16 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>morpho\morpho-v1-main\src\compound\libraries\CompoundMath.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/Lens.sol</v>
       </c>
       <c r="B62">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -1458,33 +1458,33 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>morpho\morpho-v1-main\src\compound\libraries\InterestRatesModel.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/LensStorage.sol</v>
       </c>
       <c r="B63">
-        <v>203</v>
+        <v>48</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>morpho\morpho-v1-main\src\compound\libraries\Types.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/MarketsLens.sol</v>
       </c>
       <c r="B64">
-        <v>94</v>
+        <v>180</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -1492,10 +1492,10 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MatchingEngine.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/RatesLens.sol</v>
       </c>
       <c r="B65">
-        <v>386</v>
+        <v>453</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>morpho\morpho-v1-main\src\compound\Morpho.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/RewardsLens.sol</v>
       </c>
       <c r="B66">
-        <v>247</v>
+        <v>181</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MorphoGovernance.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/UsersLens.sol</v>
       </c>
       <c r="B67">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -1543,70 +1543,70 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MorphoStorage.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/lens/interfaces/ILens.sol</v>
       </c>
       <c r="B68">
-        <v>76</v>
+        <v>291</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E68">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>morpho\morpho-v1-main\src\compound\MorphoUtils.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/libraries/CompoundMath.sol</v>
       </c>
       <c r="B69">
-        <v>227</v>
+        <v>53</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>morpho\morpho-v1-main\src\compound\PositionsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/libraries/InterestRatesModel.sol</v>
       </c>
       <c r="B70">
-        <v>1032</v>
+        <v>203</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>morpho\morpho-v1-main\src\compound\RewardsManager.sol</v>
+        <v>morpho/morpho-v1-main/src/compound/libraries/Types.sol</v>
       </c>
       <c r="B71">
-        <v>262</v>
+        <v>94</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">

</xml_diff>